<commit_message>
fix: units in data file
</commit_message>
<xml_diff>
--- a/finance_data/costs.xlsx
+++ b/finance_data/costs.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\Inzhenerka\dbt_scooters_finance\finance_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD9A0ED-4B96-4CE5-8FDE-702DDA245E09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AAB5E50-2712-4900-BBAD-2F090FECC5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F5CBED15-2893-4438-A97F-809C9C9087CE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Costs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -109,10 +109,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -451,7 +452,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -498,7 +499,7 @@
       <c r="B2" s="1">
         <v>250000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="3">
         <v>10000</v>
       </c>
       <c r="D2" s="1">
@@ -524,7 +525,7 @@
       <c r="B3" s="1">
         <v>250000</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="3">
         <v>10000</v>
       </c>
       <c r="D3" s="1">
@@ -550,7 +551,7 @@
       <c r="B4" s="1">
         <v>270000</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="3">
         <v>10000</v>
       </c>
       <c r="D4" s="1">

</xml_diff>